<commit_message>
Add movies and customers to database
</commit_message>
<xml_diff>
--- a/movie_database.xlsx
+++ b/movie_database.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="95">
   <si>
     <t xml:space="preserve">Customers</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t xml:space="preserve">price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">genre</t>
   </si>
   <si>
     <t xml:space="preserve">genre_id</t>
@@ -318,7 +315,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -354,19 +351,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -714,7 +698,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="40">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -751,11 +735,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -791,11 +775,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -831,19 +811,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="7" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="8" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="8" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="7" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="8" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -963,10 +939,10 @@
   <dimension ref="B2:U18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L16" activeCellId="0" sqref="L16"/>
+      <selection pane="topLeft" activeCell="N4" activeCellId="0" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.88"/>
@@ -978,13 +954,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="227.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="7.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="10.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="14.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="38.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="18.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="14.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="2.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="2.83"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1048,7 +1024,7 @@
         <v>14</v>
       </c>
       <c r="P3" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q3" s="15" t="s">
         <v>10</v>
@@ -1057,60 +1033,60 @@
         <v>11</v>
       </c>
       <c r="T3" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="U3" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="U3" s="15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="21" t="n">
+      <c r="B4" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="21" t="n">
+        <v>36466</v>
+      </c>
+      <c r="E4" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="22" t="n">
-        <v>36466</v>
-      </c>
-      <c r="E4" s="22" t="s">
+      <c r="F4" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="I4" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="24" t="n">
+      <c r="K4" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="24" t="n">
+        <v>15</v>
+      </c>
+      <c r="M4" s="24" t="n">
+        <v>8.99</v>
+      </c>
+      <c r="N4" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="J4" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="25" t="s">
+      <c r="P4" s="26" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="25" t="n">
-        <v>15</v>
-      </c>
-      <c r="M4" s="25" t="n">
-        <v>8.99</v>
-      </c>
-      <c r="N4" s="26" t="n">
+      <c r="R4" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="T4" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="P4" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="R4" s="28" t="s">
+      <c r="U4" s="24" t="s">
         <v>23</v>
-      </c>
-      <c r="T4" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="U4" s="30" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1118,25 +1094,25 @@
         <v>2</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="12" t="n">
         <v>34649</v>
       </c>
       <c r="E5" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>26</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>27</v>
       </c>
       <c r="I5" s="14" t="n">
         <v>2</v>
       </c>
       <c r="J5" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="15" t="s">
         <v>28</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>29</v>
       </c>
       <c r="L5" s="15" t="n">
         <v>3</v>
@@ -1151,66 +1127,66 @@
         <v>2</v>
       </c>
       <c r="Q5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="R5" s="18" t="s">
         <v>30</v>
-      </c>
-      <c r="R5" s="18" t="s">
-        <v>31</v>
       </c>
       <c r="T5" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="U5" s="20" t="s">
-        <v>32</v>
+      <c r="U5" s="15" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="21" t="n">
+      <c r="B6" s="20" t="n">
         <v>3</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="21" t="n">
+        <v>33529</v>
+      </c>
+      <c r="E6" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="22" t="n">
-        <v>33529</v>
-      </c>
-      <c r="E6" s="22" t="s">
+      <c r="F6" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="23" t="n">
+        <v>3</v>
+      </c>
+      <c r="J6" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="24" t="n">
+      <c r="K6" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="24" t="n">
         <v>3</v>
       </c>
-      <c r="J6" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="K6" s="25" t="s">
+      <c r="M6" s="24" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="N6" s="25" t="n">
+        <v>5</v>
+      </c>
+      <c r="P6" s="26" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="L6" s="25" t="n">
+      <c r="R6" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="T6" s="28" t="n">
         <v>3</v>
       </c>
-      <c r="M6" s="25" t="n">
-        <v>4.99</v>
-      </c>
-      <c r="N6" s="26" t="n">
-        <v>5</v>
-      </c>
-      <c r="P6" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q6" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="R6" s="28" t="s">
+      <c r="U6" s="24" t="s">
         <v>38</v>
-      </c>
-      <c r="T6" s="29" t="n">
-        <v>3</v>
-      </c>
-      <c r="U6" s="30" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1218,25 +1194,25 @@
         <v>4</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" s="12" t="n">
         <v>32779</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I7" s="14" t="n">
         <v>4</v>
       </c>
       <c r="J7" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="15" t="s">
         <v>42</v>
-      </c>
-      <c r="K7" s="15" t="s">
-        <v>43</v>
       </c>
       <c r="L7" s="15" t="n">
         <v>12</v>
@@ -1251,60 +1227,60 @@
         <v>4</v>
       </c>
       <c r="Q7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="R7" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="R7" s="18" t="s">
+      <c r="T7" s="29" t="n">
+        <v>4</v>
+      </c>
+      <c r="U7" s="30" t="s">
         <v>45</v>
-      </c>
-      <c r="T7" s="31" t="n">
-        <v>4</v>
-      </c>
-      <c r="U7" s="32" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="21" t="n">
+      <c r="B8" s="20" t="n">
         <v>5</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="21" t="n">
+        <v>34926</v>
+      </c>
+      <c r="E8" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="22" t="n">
-        <v>34926</v>
-      </c>
-      <c r="E8" s="22" t="s">
+      <c r="F8" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="23" t="n">
+        <v>5</v>
+      </c>
+      <c r="J8" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="I8" s="24" t="n">
+      <c r="K8" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="L8" s="24" t="n">
+        <v>3</v>
+      </c>
+      <c r="M8" s="24" t="n">
+        <v>9.99</v>
+      </c>
+      <c r="N8" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="P8" s="26" t="n">
         <v>5</v>
       </c>
-      <c r="J8" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="K8" s="25" t="s">
+      <c r="Q8" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="L8" s="25" t="n">
-        <v>3</v>
-      </c>
-      <c r="M8" s="25" t="n">
-        <v>9.99</v>
-      </c>
-      <c r="N8" s="26" t="n">
-        <v>2</v>
-      </c>
-      <c r="P8" s="27" t="n">
-        <v>5</v>
-      </c>
-      <c r="Q8" s="25" t="s">
+      <c r="R8" s="27" t="s">
         <v>51</v>
-      </c>
-      <c r="R8" s="28" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1312,25 +1288,25 @@
         <v>6</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D9" s="12" t="n">
         <v>31535</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I9" s="14" t="n">
         <v>6</v>
       </c>
       <c r="J9" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="K9" s="15" t="s">
         <v>55</v>
-      </c>
-      <c r="K9" s="15" t="s">
-        <v>56</v>
       </c>
       <c r="L9" s="15" t="n">
         <v>3</v>
@@ -1341,48 +1317,48 @@
       <c r="N9" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="P9" s="33" t="n">
+      <c r="P9" s="31" t="n">
         <v>6</v>
       </c>
-      <c r="Q9" s="34" t="s">
+      <c r="Q9" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="R9" s="33" t="s">
         <v>57</v>
-      </c>
-      <c r="R9" s="35" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="21" t="n">
+      <c r="B10" s="20" t="n">
         <v>7</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="21" t="n">
+        <v>36255</v>
+      </c>
+      <c r="E10" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="22" t="n">
-        <v>36255</v>
-      </c>
-      <c r="E10" s="22" t="s">
+      <c r="F10" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="I10" s="23" t="n">
+        <v>7</v>
+      </c>
+      <c r="J10" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="I10" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="J10" s="25" t="s">
+      <c r="K10" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="K10" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="L10" s="25" t="n">
+      <c r="L10" s="24" t="n">
         <v>12</v>
       </c>
-      <c r="M10" s="25" t="n">
+      <c r="M10" s="24" t="n">
         <v>7.99</v>
       </c>
-      <c r="N10" s="26" t="n">
+      <c r="N10" s="25" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1391,25 +1367,25 @@
         <v>8</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D11" s="12" t="n">
         <v>36890</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I11" s="14" t="n">
         <v>8</v>
       </c>
       <c r="J11" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="K11" s="15" t="s">
         <v>66</v>
-      </c>
-      <c r="K11" s="15" t="s">
-        <v>67</v>
       </c>
       <c r="L11" s="15" t="n">
         <v>15</v>
@@ -1422,37 +1398,37 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="21" t="n">
+      <c r="B12" s="20" t="n">
         <v>9</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="21" t="n">
+        <v>37116</v>
+      </c>
+      <c r="E12" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="22" t="n">
-        <v>37116</v>
-      </c>
-      <c r="E12" s="22" t="s">
+      <c r="F12" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="23" t="n">
+        <v>9</v>
+      </c>
+      <c r="J12" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="F12" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="I12" s="24" t="n">
-        <v>9</v>
-      </c>
-      <c r="J12" s="25" t="s">
+      <c r="K12" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="L12" s="25" t="n">
+      <c r="L12" s="24" t="n">
         <v>15</v>
       </c>
-      <c r="M12" s="25" t="n">
+      <c r="M12" s="24" t="n">
         <v>11.99</v>
       </c>
-      <c r="N12" s="26" t="n">
+      <c r="N12" s="25" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1461,25 +1437,25 @@
         <v>10</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D13" s="12" t="n">
         <v>37286</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I13" s="14" t="n">
         <v>10</v>
       </c>
       <c r="J13" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="K13" s="15" t="s">
         <v>74</v>
-      </c>
-      <c r="K13" s="15" t="s">
-        <v>75</v>
       </c>
       <c r="L13" s="15" t="n">
         <v>15</v>
@@ -1492,37 +1468,37 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="21" t="n">
+      <c r="B14" s="20" t="n">
         <v>11</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="21" t="n">
+        <v>35772</v>
+      </c>
+      <c r="E14" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="D14" s="22" t="n">
-        <v>35772</v>
-      </c>
-      <c r="E14" s="22" t="s">
+      <c r="F14" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="23" t="n">
+        <v>11</v>
+      </c>
+      <c r="J14" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="F14" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="I14" s="24" t="n">
-        <v>11</v>
-      </c>
-      <c r="J14" s="25" t="s">
+      <c r="K14" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="K14" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="L14" s="25" t="n">
+      <c r="L14" s="24" t="n">
         <v>3</v>
       </c>
-      <c r="M14" s="25" t="n">
+      <c r="M14" s="24" t="n">
         <v>5.99</v>
       </c>
-      <c r="N14" s="26" t="n">
+      <c r="N14" s="25" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1531,25 +1507,25 @@
         <v>12</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D15" s="12" t="n">
         <v>33246</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I15" s="14" t="n">
         <v>12</v>
       </c>
       <c r="J15" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="K15" s="15" t="s">
         <v>82</v>
-      </c>
-      <c r="K15" s="15" t="s">
-        <v>83</v>
       </c>
       <c r="L15" s="15" t="n">
         <v>3</v>
@@ -1562,37 +1538,37 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="21" t="n">
+      <c r="B16" s="20" t="n">
         <v>13</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="21" t="n">
+        <v>36679</v>
+      </c>
+      <c r="E16" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="D16" s="22" t="n">
-        <v>36679</v>
-      </c>
-      <c r="E16" s="22" t="s">
+      <c r="F16" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="23" t="n">
+        <v>13</v>
+      </c>
+      <c r="J16" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="F16" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="I16" s="24" t="n">
-        <v>13</v>
-      </c>
-      <c r="J16" s="25" t="s">
+      <c r="K16" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="K16" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="L16" s="25" t="n">
+      <c r="L16" s="24" t="n">
         <v>12</v>
       </c>
-      <c r="M16" s="25" t="n">
+      <c r="M16" s="24" t="n">
         <v>7.99</v>
       </c>
-      <c r="N16" s="26" t="n">
+      <c r="N16" s="25" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1601,25 +1577,25 @@
         <v>14</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D17" s="12" t="n">
         <v>33575</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I17" s="14" t="n">
         <v>14</v>
       </c>
       <c r="J17" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="K17" s="15" t="s">
         <v>90</v>
-      </c>
-      <c r="K17" s="15" t="s">
-        <v>91</v>
       </c>
       <c r="L17" s="15" t="n">
         <v>15</v>
@@ -1632,37 +1608,37 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="36" t="n">
+      <c r="B18" s="34" t="n">
         <v>15</v>
       </c>
-      <c r="C18" s="37" t="s">
+      <c r="C18" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" s="35" t="n">
+        <v>31176</v>
+      </c>
+      <c r="E18" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="D18" s="37" t="n">
-        <v>31176</v>
-      </c>
-      <c r="E18" s="37" t="s">
+      <c r="F18" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I18" s="37" t="n">
+        <v>15</v>
+      </c>
+      <c r="J18" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="F18" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="I18" s="39" t="n">
-        <v>15</v>
-      </c>
-      <c r="J18" s="40" t="s">
+      <c r="K18" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="K18" s="40" t="s">
-        <v>95</v>
-      </c>
-      <c r="L18" s="40" t="n">
+      <c r="L18" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="M18" s="40" t="n">
+      <c r="M18" s="38" t="n">
         <v>4.99</v>
       </c>
-      <c r="N18" s="41" t="n">
+      <c r="N18" s="39" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>